<commit_message>
Updated excel data for Cork KPI crawler
</commit_message>
<xml_diff>
--- a/Environmental/DRAXIS/Python/cork_env_emissions_kpi_once/KPI-Cork-emissions_public.xlsx
+++ b/Environmental/DRAXIS/Python/cork_env_emissions_kpi_once/KPI-Cork-emissions_public.xlsx
@@ -1,34 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\entzioni\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\entzioni\Desktop\projects\01_CUTLER\KPIs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71E7F21-5E0F-4B18-8473-E04BBBE164A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770CAD83-EC0E-4A74-82FF-AB2F0C6E6FAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{AF3C6EDA-3C2E-4C91-A10A-A33CE366F296}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{AF3C6EDA-3C2E-4C91-A10A-A33CE366F296}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="10" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
   <si>
     <t>Year</t>
   </si>
@@ -64,6 +56,12 @@
   </si>
   <si>
     <t>Passengers</t>
+  </si>
+  <si>
+    <t>Reduced Emissions for cars (5%)</t>
+  </si>
+  <si>
+    <t>Reduced Emissions for cars (10%)</t>
   </si>
 </sst>
 </file>
@@ -527,22 +525,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{566F1A24-7056-45E3-BAD8-678277A39251}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" customWidth="1"/>
-    <col min="6" max="6" width="12.7265625" customWidth="1"/>
+    <col min="3" max="5" width="10.1796875" customWidth="1"/>
+    <col min="6" max="6" width="10.26953125" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" customWidth="1"/>
+    <col min="8" max="8" width="12.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -553,16 +551,22 @@
         <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
@@ -573,16 +577,24 @@
         <v>89.581738999999999</v>
       </c>
       <c r="D2" s="12">
+        <f>0.95*C2</f>
+        <v>85.102652049999989</v>
+      </c>
+      <c r="E2" s="12">
+        <f>0.9*C2</f>
+        <v>80.623565100000008</v>
+      </c>
+      <c r="F2" s="12">
         <v>232.00320000000002</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>3</v>
       </c>
@@ -593,16 +605,24 @@
         <v>96.157852000000005</v>
       </c>
       <c r="D3" s="12">
+        <f t="shared" ref="D3:D7" si="0">0.95*C3</f>
+        <v>91.349959400000003</v>
+      </c>
+      <c r="E3" s="12">
+        <f t="shared" ref="E3:E7" si="1">0.9*C3</f>
+        <v>86.542066800000001</v>
+      </c>
+      <c r="F3" s="12">
         <v>232.00320000000002</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
@@ -613,16 +633,24 @@
         <v>3.7350625000000006</v>
       </c>
       <c r="D4" s="13">
+        <f t="shared" si="0"/>
+        <v>3.5483093750000005</v>
+      </c>
+      <c r="E4" s="13">
+        <f t="shared" si="1"/>
+        <v>3.3615562500000005</v>
+      </c>
+      <c r="F4" s="13">
         <v>29.744</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
         <v>3</v>
       </c>
@@ -633,16 +661,24 @@
         <v>4.0092499999999998</v>
       </c>
       <c r="D5" s="13">
+        <f t="shared" si="0"/>
+        <v>3.8087874999999998</v>
+      </c>
+      <c r="E5" s="13">
+        <f t="shared" si="1"/>
+        <v>3.6083249999999998</v>
+      </c>
+      <c r="F5" s="13">
         <v>29.744</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="H5" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>2</v>
       </c>
@@ -653,16 +689,24 @@
         <v>388.6556635</v>
       </c>
       <c r="D6" s="14">
+        <f t="shared" si="0"/>
+        <v>369.22288032500001</v>
+      </c>
+      <c r="E6" s="14">
+        <f t="shared" si="1"/>
+        <v>349.79009715000001</v>
+      </c>
+      <c r="F6" s="14">
         <v>148.72</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="H6" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
         <v>3</v>
       </c>
@@ -673,12 +717,20 @@
         <v>417.18651799999998</v>
       </c>
       <c r="D7" s="14">
+        <f t="shared" si="0"/>
+        <v>396.32719209999993</v>
+      </c>
+      <c r="E7" s="14">
+        <f t="shared" si="1"/>
+        <v>375.4678662</v>
+      </c>
+      <c r="F7" s="14">
         <v>148.72</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="H7" s="7" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>